<commit_message>
Updated table 1 with changed missing
</commit_message>
<xml_diff>
--- a/results/table_1.xlsx
+++ b/results/table_1.xlsx
@@ -717,17 +717,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4 (0%)</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3 (1%)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1 (0%)</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -790,17 +790,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8 (0%)</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3 (1%)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5 (0%)</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -885,17 +885,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3 (0%)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1 (0%)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2 (0%)</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -914,17 +914,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>415 (19%)</t>
+          <t>415 (56%)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>112 (22%)</t>
+          <t>112 (46%)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>303 (18%)</t>
+          <t>303 (60%)</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>203 (9%)</t>
+          <t>203 (27%)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>82 (16%)</t>
+          <t>82 (34%)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>121 (7%)</t>
+          <t>121 (24%)</t>
         </is>
       </c>
     </row>
@@ -958,17 +958,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>104 (5%)</t>
+          <t>104 (14%)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>38 (7%)</t>
+          <t>38 (16%)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>66 (4%)</t>
+          <t>66 (13%)</t>
         </is>
       </c>
     </row>
@@ -980,17 +980,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>21 (1%)</t>
+          <t>21 (3%)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>9 (2%)</t>
+          <t>9 (4%)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12 (1%)</t>
+          <t>12 (2%)</t>
         </is>
       </c>
     </row>
@@ -1002,17 +1002,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,411 (66%)</t>
+          <t>1,411</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>267 (53%)</t>
+          <t>267</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1,144 (70%)</t>
+          <t>1,144</t>
         </is>
       </c>
     </row>
@@ -1097,17 +1097,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2 (0%)</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1 (0%)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1 (0%)</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6%</t>
+          <t>7%</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>71,192</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>33,682</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>37,510</t>
         </is>
       </c>
     </row>
@@ -1534,12 +1534,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1556,17 +1556,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>292,666</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>196,914</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95,752</t>
         </is>
       </c>
     </row>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>55,579</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9,230</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>46,348</t>
         </is>
       </c>
     </row>
@@ -1680,17 +1680,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>66%</t>
         </is>
       </c>
     </row>
@@ -1702,17 +1702,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>22%</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>13%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>6%</t>
+          <t>20%</t>
         </is>
       </c>
     </row>
@@ -1724,17 +1724,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>13%</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>11%</t>
         </is>
       </c>
     </row>
@@ -1746,17 +1746,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>2%</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1%</t>
         </is>
       </c>
     </row>
@@ -1768,17 +1768,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>48,238,432</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>7,992,154</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>40,246,278</t>
         </is>
       </c>
     </row>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1863,17 +1863,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>105,951</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>40,321</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>65,630</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the confounder list
</commit_message>
<xml_diff>
--- a/results/table_1.xlsx
+++ b/results/table_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sachijay_student_ubc_ca/Documents/courses/spph_604_application_of_advanced_epidemiological_methods/spph604_final_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_57D88B8D41A37F99E6C558510B7ECD36AB4B24C9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{377C4449-3180-48B3-8668-39D1A7A1166D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_6D482A96C94375EC242451510BE88DB18851F494" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25DE3C40-9099-443E-B299-240B5AB0F86B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unadjusted" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="142">
   <si>
     <t>**Characteristic**</t>
   </si>
@@ -41,25 +41,25 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>1,854 (86%)</t>
-  </si>
-  <si>
-    <t>451 (89%)</t>
-  </si>
-  <si>
-    <t>1,403 (85%)</t>
+    <t>1,854</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>1,403</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>300 (14%)</t>
-  </si>
-  <si>
-    <t>57 (11%)</t>
-  </si>
-  <si>
-    <t>243 (15%)</t>
+    <t>300</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>243</t>
   </si>
   <si>
     <t>Age (years)</t>
@@ -80,168 +80,72 @@
     <t>Male</t>
   </si>
   <si>
-    <t>904 (42%)</t>
-  </si>
-  <si>
-    <t>204 (40%)</t>
-  </si>
-  <si>
-    <t>700 (43%)</t>
+    <t>904</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>700</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>1,250 (58%)</t>
-  </si>
-  <si>
-    <t>304 (60%)</t>
-  </si>
-  <si>
-    <t>946 (57%)</t>
-  </si>
-  <si>
-    <t>No. of healthcare visits</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>263 (12%)</t>
-  </si>
-  <si>
-    <t>35 (7%)</t>
-  </si>
-  <si>
-    <t>228 (14%)</t>
+    <t>1,250</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>946</t>
+  </si>
+  <si>
+    <t>Income ratio</t>
+  </si>
+  <si>
+    <t>1.9 (1.0, 3.9)</t>
+  </si>
+  <si>
+    <t>1.4 (0.9, 2.5)</t>
+  </si>
+  <si>
+    <t>2.2 (1.1, 4.2)</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>261</t>
+  </si>
+  <si>
+    <t>Lung cancer</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>268 (12%)</t>
-  </si>
-  <si>
-    <t>233 (14%)</t>
-  </si>
-  <si>
-    <t>2 to 3</t>
-  </si>
-  <si>
-    <t>582 (27%)</t>
-  </si>
-  <si>
-    <t>100 (20%)</t>
-  </si>
-  <si>
-    <t>482 (29%)</t>
-  </si>
-  <si>
-    <t>4 to 5</t>
-  </si>
-  <si>
-    <t>393 (18%)</t>
-  </si>
-  <si>
-    <t>95 (19%)</t>
-  </si>
-  <si>
-    <t>298 (18%)</t>
-  </si>
-  <si>
-    <t>6 to 7</t>
-  </si>
-  <si>
-    <t>190 (9%)</t>
-  </si>
-  <si>
-    <t>63 (12%)</t>
-  </si>
-  <si>
-    <t>127 (8%)</t>
-  </si>
-  <si>
-    <t>8 to 9</t>
-  </si>
-  <si>
-    <t>91 (4%)</t>
-  </si>
-  <si>
-    <t>29 (6%)</t>
-  </si>
-  <si>
-    <t>62 (4%)</t>
-  </si>
-  <si>
-    <t>10 to 12</t>
-  </si>
-  <si>
-    <t>162 (8%)</t>
-  </si>
-  <si>
-    <t>58 (11%)</t>
-  </si>
-  <si>
-    <t>104 (6%)</t>
-  </si>
-  <si>
-    <t>13 to 15</t>
-  </si>
-  <si>
-    <t>56 (3%)</t>
-  </si>
-  <si>
-    <t>25 (5%)</t>
-  </si>
-  <si>
-    <t>31 (2%)</t>
-  </si>
-  <si>
-    <t>16 or more</t>
-  </si>
-  <si>
-    <t>145 (7%)</t>
-  </si>
-  <si>
-    <t>65 (13%)</t>
-  </si>
-  <si>
-    <t>80 (5%)</t>
-  </si>
-  <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>2,131</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>1,640</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Lung cancer</t>
-  </si>
-  <si>
-    <t>15 (1%)</t>
-  </si>
-  <si>
-    <t>14 (3%)</t>
-  </si>
-  <si>
-    <t>1 (0%)</t>
-  </si>
-  <si>
-    <t>2,131 (99%)</t>
-  </si>
-  <si>
-    <t>491 (97%)</t>
-  </si>
-  <si>
-    <t>1,640 (100%)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -251,37 +155,37 @@
     <t>Current smokers</t>
   </si>
   <si>
-    <t>486 (23%)</t>
-  </si>
-  <si>
-    <t>190 (37%)</t>
-  </si>
-  <si>
-    <t>296 (18%)</t>
+    <t>486</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>296</t>
   </si>
   <si>
     <t>Former smokers</t>
   </si>
   <si>
-    <t>520 (24%)</t>
-  </si>
-  <si>
-    <t>156 (31%)</t>
-  </si>
-  <si>
-    <t>364 (22%)</t>
+    <t>520</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>364</t>
   </si>
   <si>
     <t>Never smoked</t>
   </si>
   <si>
-    <t>1,145 (53%)</t>
-  </si>
-  <si>
-    <t>161 (32%)</t>
-  </si>
-  <si>
-    <t>984 (60%)</t>
+    <t>1,145</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>984</t>
   </si>
   <si>
     <t>2</t>
@@ -293,40 +197,40 @@
     <t>0</t>
   </si>
   <si>
-    <t>415 (56%)</t>
-  </si>
-  <si>
-    <t>112 (46%)</t>
-  </si>
-  <si>
-    <t>303 (60%)</t>
-  </si>
-  <si>
-    <t>203 (27%)</t>
-  </si>
-  <si>
-    <t>82 (34%)</t>
-  </si>
-  <si>
-    <t>121 (24%)</t>
-  </si>
-  <si>
-    <t>104 (14%)</t>
-  </si>
-  <si>
-    <t>38 (16%)</t>
-  </si>
-  <si>
-    <t>66 (13%)</t>
-  </si>
-  <si>
-    <t>21 (3%)</t>
-  </si>
-  <si>
-    <t>9 (4%)</t>
-  </si>
-  <si>
-    <t>12 (2%)</t>
+    <t>415</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>1,411</t>
@@ -341,31 +245,31 @@
     <t>Has diabetes</t>
   </si>
   <si>
-    <t>381 (18%)</t>
-  </si>
-  <si>
-    <t>153 (30%)</t>
-  </si>
-  <si>
-    <t>1,714 (80%)</t>
-  </si>
-  <si>
-    <t>336 (66%)</t>
-  </si>
-  <si>
-    <t>1,378 (84%)</t>
+    <t>381</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>1,714</t>
+  </si>
+  <si>
+    <t>336</t>
+  </si>
+  <si>
+    <t>1,378</t>
   </si>
   <si>
     <t>Borderline</t>
   </si>
   <si>
-    <t>57 (3%)</t>
-  </si>
-  <si>
-    <t>18 (4%)</t>
-  </si>
-  <si>
-    <t>39 (2%)</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
   <si>
     <t>88%</t>
@@ -413,25 +317,94 @@
     <t>55%</t>
   </si>
   <si>
-    <t>6%</t>
-  </si>
-  <si>
-    <t>14%</t>
-  </si>
-  <si>
-    <t>8%</t>
-  </si>
-  <si>
-    <t>15%</t>
+    <t>2.8 (1.3, 4.9)</t>
+  </si>
+  <si>
+    <t>1.8 (0.9, 3.5)</t>
+  </si>
+  <si>
+    <t>3.1 (1.6, 5.0)</t>
+  </si>
+  <si>
+    <t>7,311,139</t>
+  </si>
+  <si>
+    <t>1,342,317</t>
+  </si>
+  <si>
+    <t>5,968,821</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>98%</t>
+  </si>
+  <si>
+    <t>292,666</t>
+  </si>
+  <si>
+    <t>196,914</t>
+  </si>
+  <si>
+    <t>95,752</t>
+  </si>
+  <si>
+    <t>21%</t>
+  </si>
+  <si>
+    <t>37%</t>
+  </si>
+  <si>
+    <t>17%</t>
+  </si>
+  <si>
+    <t>27%</t>
+  </si>
+  <si>
+    <t>31%</t>
+  </si>
+  <si>
+    <t>26%</t>
+  </si>
+  <si>
+    <t>51%</t>
+  </si>
+  <si>
+    <t>56%</t>
+  </si>
+  <si>
+    <t>55,579</t>
+  </si>
+  <si>
+    <t>9,230</t>
+  </si>
+  <si>
+    <t>46,348</t>
+  </si>
+  <si>
+    <t>62%</t>
+  </si>
+  <si>
+    <t>52%</t>
+  </si>
+  <si>
+    <t>66%</t>
+  </si>
+  <si>
+    <t>22%</t>
   </si>
   <si>
     <t>28%</t>
   </si>
   <si>
-    <t>23%</t>
-  </si>
-  <si>
-    <t>30%</t>
+    <t>20%</t>
   </si>
   <si>
     <t>16%</t>
@@ -440,88 +413,10 @@
     <t>11%</t>
   </si>
   <si>
+    <t>3%</t>
+  </si>
+  <si>
     <t>4%</t>
-  </si>
-  <si>
-    <t>7%</t>
-  </si>
-  <si>
-    <t>3%</t>
-  </si>
-  <si>
-    <t>2%</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>71,192</t>
-  </si>
-  <si>
-    <t>33,682</t>
-  </si>
-  <si>
-    <t>37,510</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>292,666</t>
-  </si>
-  <si>
-    <t>196,914</t>
-  </si>
-  <si>
-    <t>95,752</t>
-  </si>
-  <si>
-    <t>21%</t>
-  </si>
-  <si>
-    <t>37%</t>
-  </si>
-  <si>
-    <t>17%</t>
-  </si>
-  <si>
-    <t>27%</t>
-  </si>
-  <si>
-    <t>31%</t>
-  </si>
-  <si>
-    <t>26%</t>
-  </si>
-  <si>
-    <t>51%</t>
-  </si>
-  <si>
-    <t>56%</t>
-  </si>
-  <si>
-    <t>55,579</t>
-  </si>
-  <si>
-    <t>9,230</t>
-  </si>
-  <si>
-    <t>46,348</t>
-  </si>
-  <si>
-    <t>62%</t>
-  </si>
-  <si>
-    <t>52%</t>
-  </si>
-  <si>
-    <t>66%</t>
-  </si>
-  <si>
-    <t>22%</t>
-  </si>
-  <si>
-    <t>20%</t>
   </si>
   <si>
     <t>48,238,432</t>
@@ -595,12 +490,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,403 +911,285 @@
       <c r="A9" t="s">
         <v>26</v>
       </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,13 +1224,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,13 +1238,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,13 +1252,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,13 +1271,13 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,406 +1285,288 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
         <v>141</v>
-      </c>
-      <c r="C33" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>172</v>
-      </c>
-      <c r="C37" t="s">
-        <v>173</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" t="s">
-        <v>142</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>174</v>
-      </c>
-      <c r="C39" t="s">
-        <v>175</v>
-      </c>
-      <c r="D39" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated table 1 export
</commit_message>
<xml_diff>
--- a/results/table_1.xlsx
+++ b/results/table_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sachijay_student_ubc_ca/Documents/courses/spph_604_application_of_advanced_epidemiological_methods/spph604_final_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6D482A96C94375EC242451510BE88DB18851F494" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25DE3C40-9099-443E-B299-240B5AB0F86B}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_6D482A96C94375EC242451510BE88DB18851F494" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D81544EF-4508-4FF6-975D-FD487817881A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unadjusted" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
   <si>
     <t>**Characteristic**</t>
   </si>
@@ -510,6 +510,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,7 +806,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,8 +935,8 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
+      <c r="D10">
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>